<commit_message>
- Alteração do fluxo de abertura e fechamento da O.S. - Correções dos selos/lacres. Agora o técnico só pode ver os selos/lacres (não pode lançar); - Só são puxados na O.S os Selos/Lacres pertencentes ao técnico e que ainda não foram utilizados.
</commit_message>
<xml_diff>
--- a/storage/uploads/import/import.xlsx
+++ b/storage/uploads/import/import.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\workana\atlas\storage\uploads\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\workana\gestaoatlas\storage\uploads\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="210" windowWidth="16425" windowHeight="7935" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="2625" yWindow="210" windowWidth="16425" windowHeight="7935" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="11" r:id="rId1"/>
@@ -754,17 +754,17 @@
       <selection activeCell="F1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="3" width="39.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="10.25" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="6" customWidth="1"/>
+    <col min="2" max="3" width="39.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="6" customWidth="1"/>
     <col min="9" max="9" width="9" style="6"/>
-    <col min="10" max="10" width="10.625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -859,16 +859,16 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -907,20 +907,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1004,16 +1004,16 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1061,16 +1061,16 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="71.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1134,20 +1134,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1163,17 +1163,17 @@
     </row>
     <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -1200,17 +1200,17 @@
       <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="39.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
-    <col min="9" max="9" width="10.625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1260,17 +1260,17 @@
       <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="39.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
-    <col min="9" max="9" width="10.625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1320,17 +1320,17 @@
       <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="39.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
-    <col min="9" max="9" width="10.625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1380,17 +1380,17 @@
       <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="39.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="6" customWidth="1"/>
     <col min="8" max="8" width="9" style="6"/>
-    <col min="9" max="9" width="10.625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="6" customWidth="1"/>
     <col min="10" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1456,16 +1456,16 @@
       <selection activeCell="A5" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1508,16 +1508,16 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1580,16 +1580,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1627,16 +1627,16 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="9" style="6"/>
-    <col min="8" max="8" width="10.625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
- Inclusão da importação das peças
</commit_message>
<xml_diff>
--- a/storage/uploads/import/import.xlsx
+++ b/storage/uploads/import/import.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="210" windowWidth="16425" windowHeight="7935" firstSheet="3" activeTab="13"/>
+    <workbookView xWindow="2625" yWindow="210" windowWidth="16425" windowHeight="7935" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="11" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
   <si>
     <t>FILIZOLA</t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>Descrição do Serviço 5</t>
+  </si>
+  <si>
+    <t>unid</t>
+  </si>
+  <si>
+    <t>UNIDADE</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1374,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,6 +1446,14 @@
       </c>
       <c r="B6" s="2" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>